<commit_message>
Restauration complète + ajout GEKA
</commit_message>
<xml_diff>
--- a/prix/pex.xlsx
+++ b/prix/pex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\raccords-plomberie\prix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94CA6333-18DC-4CFD-897C-D498C5552551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE5FB7D-973A-461F-8D71-A0B530FB9878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C27940F6-7049-4028-8D53-A9BC0C24D70B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="321">
   <si>
     <t>43122970</t>
   </si>
@@ -896,9 +896,6 @@
     <t>26</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>16-1/2</t>
   </si>
   <si>
@@ -906,6 +903,102 @@
   </si>
   <si>
     <t>20 -2</t>
+  </si>
+  <si>
+    <t>pex/bouchon.png</t>
+  </si>
+  <si>
+    <t>pex/coude-f-el.png</t>
+  </si>
+  <si>
+    <t>pex/coude-femelle.png</t>
+  </si>
+  <si>
+    <t>pex/coude-male.png</t>
+  </si>
+  <si>
+    <t>pex/culasse-doucle.png</t>
+  </si>
+  <si>
+    <t>pex/culasse-simple.png</t>
+  </si>
+  <si>
+    <t>pex/manchon.png</t>
+  </si>
+  <si>
+    <t>pex/pex-coude.png</t>
+  </si>
+  <si>
+    <t>pex/raccord-f-el.png</t>
+  </si>
+  <si>
+    <t>pex/raccord-femelle.png</t>
+  </si>
+  <si>
+    <t>pex/raccord-male.png</t>
+  </si>
+  <si>
+    <t>pex/te-femelle.png</t>
+  </si>
+  <si>
+    <t>pex/te-male.png</t>
+  </si>
+  <si>
+    <t>pex/te-reduit.png</t>
+  </si>
+  <si>
+    <t>pex/te.png</t>
+  </si>
+  <si>
+    <t>pex/vanne.png</t>
+  </si>
+  <si>
+    <t>pex-a-sertir/bouchon.png</t>
+  </si>
+  <si>
+    <t>pex-a-sertir/coude-egal.png</t>
+  </si>
+  <si>
+    <t>pex-a-sertir/coude-femelle-el.png</t>
+  </si>
+  <si>
+    <t>pex-a-sertir/coude-femelle.png</t>
+  </si>
+  <si>
+    <t>pex-a-sertir/coude-male.png</t>
+  </si>
+  <si>
+    <t>pex-a-sertir/culasse-double.png</t>
+  </si>
+  <si>
+    <t>pex-a-sertir/culasse-simple.png</t>
+  </si>
+  <si>
+    <t>2S</t>
+  </si>
+  <si>
+    <t>pex-a-sertir/manchon.png</t>
+  </si>
+  <si>
+    <t>pex-a-sertir/rac-femelle-el.png</t>
+  </si>
+  <si>
+    <t>pex-a-sertir/raccord-femelle.png</t>
+  </si>
+  <si>
+    <t>pex-a-sertir/raccord-male.png</t>
+  </si>
+  <si>
+    <t>pex-a-sertir/te-egal.png</t>
+  </si>
+  <si>
+    <t>pex-a-sertir/te-femelle.png</t>
+  </si>
+  <si>
+    <t>pex-a-sertir/te-male.png</t>
+  </si>
+  <si>
+    <t>pex-a-sertir/te-reduit.png</t>
   </si>
 </sst>
 </file>
@@ -1316,13 +1409,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11EDDEF9-0BC9-4BCE-BC53-B53A6E5EDDA0}">
   <dimension ref="A1:K129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="A83" sqref="A83:A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" style="7"/>
+    <col min="1" max="1" width="28.5546875" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.44140625" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.44140625" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" style="7" bestFit="1" customWidth="1"/>
@@ -1357,6 +1450,9 @@
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>291</v>
+      </c>
       <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
@@ -1371,6 +1467,9 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>291</v>
+      </c>
       <c r="B3" s="8" t="s">
         <v>3</v>
       </c>
@@ -1385,6 +1484,9 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>291</v>
+      </c>
       <c r="B4" s="8" t="s">
         <v>5</v>
       </c>
@@ -1399,6 +1501,9 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>292</v>
+      </c>
       <c r="B5" s="8" t="s">
         <v>7</v>
       </c>
@@ -1413,6 +1518,9 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>292</v>
+      </c>
       <c r="B6" s="8" t="s">
         <v>9</v>
       </c>
@@ -1427,6 +1535,9 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>292</v>
+      </c>
       <c r="B7" s="8" t="s">
         <v>11</v>
       </c>
@@ -1441,6 +1552,9 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="B8" s="8" t="s">
         <v>13</v>
       </c>
@@ -1455,6 +1569,9 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="B9" s="8" t="s">
         <v>15</v>
       </c>
@@ -1469,6 +1586,9 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="B10" s="8" t="s">
         <v>17</v>
       </c>
@@ -1483,6 +1603,9 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>297</v>
+      </c>
       <c r="B11" s="8" t="s">
         <v>19</v>
       </c>
@@ -1497,6 +1620,9 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>297</v>
+      </c>
       <c r="B12" s="8" t="s">
         <v>21</v>
       </c>
@@ -1511,6 +1637,9 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>297</v>
+      </c>
       <c r="B13" s="8" t="s">
         <v>23</v>
       </c>
@@ -1525,6 +1654,9 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>297</v>
+      </c>
       <c r="B14" s="8" t="s">
         <v>25</v>
       </c>
@@ -1539,6 +1671,9 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>297</v>
+      </c>
       <c r="B15" s="8" t="s">
         <v>27</v>
       </c>
@@ -1613,7 +1748,7 @@
         <v>37</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D20" s="9">
         <v>52.13</v>
@@ -1627,7 +1762,7 @@
         <v>39</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D21" s="9">
         <v>52.13</v>
@@ -1786,7 +1921,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B33" s="8" t="s">
         <v>63</v>
       </c>
@@ -1800,7 +1935,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B34" s="8" t="s">
         <v>65</v>
       </c>
@@ -1814,7 +1949,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B35" s="8" t="s">
         <v>67</v>
       </c>
@@ -1826,7 +1961,10 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="7" t="s">
+        <v>299</v>
+      </c>
       <c r="B36" s="8" t="s">
         <v>69</v>
       </c>
@@ -1840,7 +1978,10 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="7" t="s">
+        <v>299</v>
+      </c>
       <c r="B37" s="8" t="s">
         <v>71</v>
       </c>
@@ -1854,7 +1995,10 @@
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="7" t="s">
+        <v>299</v>
+      </c>
       <c r="B38" s="8" t="s">
         <v>73</v>
       </c>
@@ -1868,7 +2012,10 @@
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="7" t="s">
+        <v>299</v>
+      </c>
       <c r="B39" s="8" t="s">
         <v>75</v>
       </c>
@@ -1882,7 +2029,10 @@
         <v>74</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="7" t="s">
+        <v>299</v>
+      </c>
       <c r="B40" s="8" t="s">
         <v>77</v>
       </c>
@@ -1896,7 +2046,10 @@
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="7" t="s">
+        <v>298</v>
+      </c>
       <c r="B41" s="8" t="s">
         <v>79</v>
       </c>
@@ -1910,7 +2063,10 @@
         <v>78</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="7" t="s">
+        <v>298</v>
+      </c>
       <c r="B42" s="8" t="s">
         <v>81</v>
       </c>
@@ -1924,7 +2080,10 @@
         <v>80</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="7" t="s">
+        <v>298</v>
+      </c>
       <c r="B43" s="8" t="s">
         <v>83</v>
       </c>
@@ -1938,7 +2097,10 @@
         <v>82</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="7" t="s">
+        <v>298</v>
+      </c>
       <c r="B44" s="8" t="s">
         <v>85</v>
       </c>
@@ -1952,7 +2114,10 @@
         <v>84</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="7" t="s">
+        <v>298</v>
+      </c>
       <c r="B45" s="8" t="s">
         <v>87</v>
       </c>
@@ -1966,7 +2131,10 @@
         <v>86</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="7" t="s">
+        <v>303</v>
+      </c>
       <c r="B46" s="8" t="s">
         <v>89</v>
       </c>
@@ -1980,7 +2148,10 @@
         <v>88</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="7" t="s">
+        <v>303</v>
+      </c>
       <c r="B47" s="8" t="s">
         <v>91</v>
       </c>
@@ -1992,7 +2163,10 @@
         <v>90</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="7" t="s">
+        <v>303</v>
+      </c>
       <c r="B48" s="8" t="s">
         <v>93</v>
       </c>
@@ -2006,7 +2180,10 @@
         <v>92</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="7" t="s">
+        <v>300</v>
+      </c>
       <c r="B49" s="8" t="s">
         <v>95</v>
       </c>
@@ -2020,7 +2197,10 @@
         <v>94</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="7" t="s">
+        <v>300</v>
+      </c>
       <c r="B50" s="8" t="s">
         <v>97</v>
       </c>
@@ -2034,7 +2214,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B51" s="8" t="s">
         <v>99</v>
       </c>
@@ -2046,7 +2226,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B52" s="8" t="s">
         <v>101</v>
       </c>
@@ -2058,7 +2238,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="7" t="s">
+        <v>301</v>
+      </c>
       <c r="B53" s="8" t="s">
         <v>103</v>
       </c>
@@ -2072,7 +2255,10 @@
         <v>102</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" s="7" t="s">
+        <v>301</v>
+      </c>
       <c r="B54" s="8" t="s">
         <v>105</v>
       </c>
@@ -2086,7 +2272,10 @@
         <v>104</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" s="7" t="s">
+        <v>302</v>
+      </c>
       <c r="B55" s="8" t="s">
         <v>107</v>
       </c>
@@ -2100,7 +2289,10 @@
         <v>106</v>
       </c>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" s="7" t="s">
+        <v>302</v>
+      </c>
       <c r="B56" s="8" t="s">
         <v>109</v>
       </c>
@@ -2114,7 +2306,10 @@
         <v>108</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" s="7" t="s">
+        <v>302</v>
+      </c>
       <c r="B57" s="8" t="s">
         <v>111</v>
       </c>
@@ -2128,7 +2323,10 @@
         <v>110</v>
       </c>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" s="7" t="s">
+        <v>296</v>
+      </c>
       <c r="B58" s="8" t="s">
         <v>113</v>
       </c>
@@ -2140,7 +2338,10 @@
         <v>112</v>
       </c>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" s="7" t="s">
+        <v>296</v>
+      </c>
       <c r="B59" s="8" t="s">
         <v>115</v>
       </c>
@@ -2152,7 +2353,10 @@
         <v>114</v>
       </c>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" s="7" t="s">
+        <v>296</v>
+      </c>
       <c r="B60" s="8" t="s">
         <v>117</v>
       </c>
@@ -2164,7 +2368,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" s="7" t="s">
+        <v>293</v>
+      </c>
       <c r="B61" s="8" t="s">
         <v>119</v>
       </c>
@@ -2178,7 +2385,10 @@
         <v>118</v>
       </c>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" s="7" t="s">
+        <v>294</v>
+      </c>
       <c r="B62" s="8" t="s">
         <v>121</v>
       </c>
@@ -2192,7 +2402,10 @@
         <v>120</v>
       </c>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" s="7" t="s">
+        <v>294</v>
+      </c>
       <c r="B63" s="8" t="s">
         <v>123</v>
       </c>
@@ -2206,7 +2419,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B64" s="8" t="s">
         <v>125</v>
       </c>
@@ -2220,7 +2433,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B65" s="8" t="s">
         <v>127</v>
       </c>
@@ -2234,7 +2447,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B66" s="8" t="s">
         <v>129</v>
       </c>
@@ -2248,7 +2461,10 @@
         <v>128</v>
       </c>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" s="7" t="s">
+        <v>295</v>
+      </c>
       <c r="B67" s="8" t="s">
         <v>131</v>
       </c>
@@ -2262,7 +2478,10 @@
         <v>130</v>
       </c>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" s="7" t="s">
+        <v>295</v>
+      </c>
       <c r="B68" s="8" t="s">
         <v>133</v>
       </c>
@@ -2276,7 +2495,10 @@
         <v>132</v>
       </c>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" s="7" t="s">
+        <v>295</v>
+      </c>
       <c r="B69" s="8" t="s">
         <v>135</v>
       </c>
@@ -2290,7 +2512,10 @@
         <v>134</v>
       </c>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" s="7" t="s">
+        <v>289</v>
+      </c>
       <c r="B70" s="8" t="s">
         <v>137</v>
       </c>
@@ -2304,7 +2529,10 @@
         <v>136</v>
       </c>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" s="7" t="s">
+        <v>289</v>
+      </c>
       <c r="B71" s="8" t="s">
         <v>139</v>
       </c>
@@ -2318,7 +2546,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B72" s="8" t="s">
         <v>141</v>
       </c>
@@ -2332,7 +2560,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B73" s="8" t="s">
         <v>143</v>
       </c>
@@ -2346,7 +2574,10 @@
         <v>142</v>
       </c>
     </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74" s="7" t="s">
+        <v>311</v>
+      </c>
       <c r="B74" s="8" t="s">
         <v>145</v>
       </c>
@@ -2360,12 +2591,15 @@
         <v>144</v>
       </c>
     </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75" s="7" t="s">
+        <v>311</v>
+      </c>
       <c r="B75" s="8" t="s">
         <v>147</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>286</v>
+        <v>312</v>
       </c>
       <c r="D75" s="9">
         <v>15.82</v>
@@ -2374,12 +2608,15 @@
         <v>146</v>
       </c>
     </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76" s="7" t="s">
+        <v>310</v>
+      </c>
       <c r="B76" s="8" t="s">
         <v>149</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D76" s="9">
         <v>19.3</v>
@@ -2388,7 +2625,10 @@
         <v>148</v>
       </c>
     </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77" s="7" t="s">
+        <v>318</v>
+      </c>
       <c r="B77" s="8" t="s">
         <v>151</v>
       </c>
@@ -2402,7 +2642,10 @@
         <v>150</v>
       </c>
     </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A78" s="7" t="s">
+        <v>318</v>
+      </c>
       <c r="B78" s="8" t="s">
         <v>153</v>
       </c>
@@ -2416,7 +2659,10 @@
         <v>152</v>
       </c>
     </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A79" s="7" t="s">
+        <v>318</v>
+      </c>
       <c r="B79" s="8" t="s">
         <v>155</v>
       </c>
@@ -2430,7 +2676,10 @@
         <v>154</v>
       </c>
     </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A80" s="7" t="s">
+        <v>317</v>
+      </c>
       <c r="B80" s="8" t="s">
         <v>157</v>
       </c>
@@ -2444,7 +2693,10 @@
         <v>156</v>
       </c>
     </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81" s="7" t="s">
+        <v>317</v>
+      </c>
       <c r="B81" s="8" t="s">
         <v>159</v>
       </c>
@@ -2458,7 +2710,10 @@
         <v>158</v>
       </c>
     </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A82" s="7" t="s">
+        <v>317</v>
+      </c>
       <c r="B82" s="8" t="s">
         <v>161</v>
       </c>
@@ -2472,7 +2727,10 @@
         <v>160</v>
       </c>
     </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A83" s="7" t="s">
+        <v>320</v>
+      </c>
       <c r="B83" s="8" t="s">
         <v>163</v>
       </c>
@@ -2486,7 +2744,10 @@
         <v>162</v>
       </c>
     </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A84" s="7" t="s">
+        <v>320</v>
+      </c>
       <c r="B84" s="8" t="s">
         <v>165</v>
       </c>
@@ -2500,7 +2761,10 @@
         <v>164</v>
       </c>
     </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A85" s="7" t="s">
+        <v>320</v>
+      </c>
       <c r="B85" s="8" t="s">
         <v>167</v>
       </c>
@@ -2514,7 +2778,10 @@
         <v>166</v>
       </c>
     </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A86" s="7" t="s">
+        <v>313</v>
+      </c>
       <c r="B86" s="8" t="s">
         <v>169</v>
       </c>
@@ -2528,7 +2795,10 @@
         <v>168</v>
       </c>
     </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A87" s="7" t="s">
+        <v>313</v>
+      </c>
       <c r="B87" s="8" t="s">
         <v>171</v>
       </c>
@@ -2542,7 +2812,10 @@
         <v>170</v>
       </c>
     </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A88" s="7" t="s">
+        <v>313</v>
+      </c>
       <c r="B88" s="8" t="s">
         <v>173</v>
       </c>
@@ -2556,7 +2829,10 @@
         <v>172</v>
       </c>
     </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A89" s="7" t="s">
+        <v>316</v>
+      </c>
       <c r="B89" s="8" t="s">
         <v>175</v>
       </c>
@@ -2570,7 +2846,10 @@
         <v>174</v>
       </c>
     </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A90" s="7" t="s">
+        <v>316</v>
+      </c>
       <c r="B90" s="8" t="s">
         <v>177</v>
       </c>
@@ -2584,7 +2863,10 @@
         <v>176</v>
       </c>
     </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A91" s="7" t="s">
+        <v>316</v>
+      </c>
       <c r="B91" s="8" t="s">
         <v>179</v>
       </c>
@@ -2598,7 +2880,10 @@
         <v>178</v>
       </c>
     </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A92" s="7" t="s">
+        <v>316</v>
+      </c>
       <c r="B92" s="8" t="s">
         <v>181</v>
       </c>
@@ -2612,7 +2897,10 @@
         <v>180</v>
       </c>
     </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A93" s="7" t="s">
+        <v>316</v>
+      </c>
       <c r="B93" s="8" t="s">
         <v>183</v>
       </c>
@@ -2626,7 +2914,10 @@
         <v>182</v>
       </c>
     </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A94" s="7" t="s">
+        <v>314</v>
+      </c>
       <c r="B94" s="8" t="s">
         <v>185</v>
       </c>
@@ -2640,7 +2931,10 @@
         <v>184</v>
       </c>
     </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A95" s="7" t="s">
+        <v>314</v>
+      </c>
       <c r="B95" s="8" t="s">
         <v>187</v>
       </c>
@@ -2654,7 +2948,10 @@
         <v>186</v>
       </c>
     </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A96" s="7" t="s">
+        <v>314</v>
+      </c>
       <c r="B96" s="8" t="s">
         <v>189</v>
       </c>
@@ -2668,7 +2965,10 @@
         <v>188</v>
       </c>
     </row>
-    <row r="97" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A97" s="7" t="s">
+        <v>314</v>
+      </c>
       <c r="B97" s="8" t="s">
         <v>191</v>
       </c>
@@ -2682,7 +2982,10 @@
         <v>190</v>
       </c>
     </row>
-    <row r="98" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A98" s="7" t="s">
+        <v>314</v>
+      </c>
       <c r="B98" s="8" t="s">
         <v>193</v>
       </c>
@@ -2696,7 +2999,10 @@
         <v>192</v>
       </c>
     </row>
-    <row r="99" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A99" s="7" t="s">
+        <v>307</v>
+      </c>
       <c r="B99" s="8" t="s">
         <v>195</v>
       </c>
@@ -2710,7 +3016,10 @@
         <v>194</v>
       </c>
     </row>
-    <row r="100" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A100" s="7" t="s">
+        <v>307</v>
+      </c>
       <c r="B100" s="8" t="s">
         <v>197</v>
       </c>
@@ -2724,7 +3033,10 @@
         <v>196</v>
       </c>
     </row>
-    <row r="101" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A101" s="7" t="s">
+        <v>307</v>
+      </c>
       <c r="B101" s="8" t="s">
         <v>199</v>
       </c>
@@ -2738,7 +3050,10 @@
         <v>198</v>
       </c>
     </row>
-    <row r="102" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A102" s="7" t="s">
+        <v>306</v>
+      </c>
       <c r="B102" s="8" t="s">
         <v>201</v>
       </c>
@@ -2752,7 +3067,10 @@
         <v>200</v>
       </c>
     </row>
-    <row r="103" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A103" s="7" t="s">
+        <v>306</v>
+      </c>
       <c r="B103" s="8" t="s">
         <v>203</v>
       </c>
@@ -2766,7 +3084,10 @@
         <v>202</v>
       </c>
     </row>
-    <row r="104" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A104" s="7" t="s">
+        <v>306</v>
+      </c>
       <c r="B104" s="8" t="s">
         <v>205</v>
       </c>
@@ -2780,7 +3101,10 @@
         <v>204</v>
       </c>
     </row>
-    <row r="105" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A105" s="7" t="s">
+        <v>309</v>
+      </c>
       <c r="B105" s="8" t="s">
         <v>207</v>
       </c>
@@ -2794,7 +3118,10 @@
         <v>206</v>
       </c>
     </row>
-    <row r="106" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A106" s="7" t="s">
+        <v>309</v>
+      </c>
       <c r="B106" s="8" t="s">
         <v>209</v>
       </c>
@@ -2808,7 +3135,10 @@
         <v>208</v>
       </c>
     </row>
-    <row r="107" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A107" s="7" t="s">
+        <v>309</v>
+      </c>
       <c r="B107" s="8" t="s">
         <v>211</v>
       </c>
@@ -2822,7 +3152,10 @@
         <v>210</v>
       </c>
     </row>
-    <row r="108" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A108" s="7" t="s">
+        <v>309</v>
+      </c>
       <c r="B108" s="8" t="s">
         <v>213</v>
       </c>
@@ -2836,7 +3169,10 @@
         <v>212</v>
       </c>
     </row>
-    <row r="109" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A109" s="7" t="s">
+        <v>308</v>
+      </c>
       <c r="B109" s="8" t="s">
         <v>215</v>
       </c>
@@ -2850,7 +3186,10 @@
         <v>214</v>
       </c>
     </row>
-    <row r="110" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A110" s="7" t="s">
+        <v>308</v>
+      </c>
       <c r="B110" s="8" t="s">
         <v>217</v>
       </c>
@@ -2864,7 +3203,10 @@
         <v>216</v>
       </c>
     </row>
-    <row r="111" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A111" s="7" t="s">
+        <v>308</v>
+      </c>
       <c r="B111" s="8" t="s">
         <v>219</v>
       </c>
@@ -2878,7 +3220,10 @@
         <v>218</v>
       </c>
     </row>
-    <row r="112" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A112" s="7" t="s">
+        <v>308</v>
+      </c>
       <c r="B112" s="8" t="s">
         <v>221</v>
       </c>
@@ -2892,7 +3237,10 @@
         <v>220</v>
       </c>
     </row>
-    <row r="113" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A113" s="7" t="s">
+        <v>305</v>
+      </c>
       <c r="B113" s="8" t="s">
         <v>223</v>
       </c>
@@ -2906,7 +3254,10 @@
         <v>222</v>
       </c>
     </row>
-    <row r="114" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A114" s="7" t="s">
+        <v>305</v>
+      </c>
       <c r="B114" s="8" t="s">
         <v>225</v>
       </c>
@@ -2920,7 +3271,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="115" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B115" s="8" t="s">
         <v>227</v>
       </c>
@@ -2934,7 +3285,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="116" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B116" s="8" t="s">
         <v>99</v>
       </c>
@@ -2944,7 +3295,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="117" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B117" s="8" t="s">
         <v>230</v>
       </c>
@@ -2958,7 +3309,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="118" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B118" s="8" t="s">
         <v>232</v>
       </c>
@@ -2972,12 +3323,12 @@
         <v>231</v>
       </c>
     </row>
-    <row r="119" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B119" s="8" t="s">
         <v>234</v>
       </c>
       <c r="C119" s="8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D119" s="9">
         <v>29.830000000000002</v>
@@ -2986,7 +3337,10 @@
         <v>233</v>
       </c>
     </row>
-    <row r="120" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A120" s="7" t="s">
+        <v>315</v>
+      </c>
       <c r="B120" s="8" t="s">
         <v>236</v>
       </c>
@@ -3000,7 +3354,10 @@
         <v>235</v>
       </c>
     </row>
-    <row r="121" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A121" s="7" t="s">
+        <v>315</v>
+      </c>
       <c r="B121" s="8" t="s">
         <v>238</v>
       </c>
@@ -3014,7 +3371,10 @@
         <v>237</v>
       </c>
     </row>
-    <row r="122" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A122" s="7" t="s">
+        <v>315</v>
+      </c>
       <c r="B122" s="8" t="s">
         <v>240</v>
       </c>
@@ -3028,7 +3388,10 @@
         <v>239</v>
       </c>
     </row>
-    <row r="123" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A123" s="7" t="s">
+        <v>315</v>
+      </c>
       <c r="B123" s="8" t="s">
         <v>242</v>
       </c>
@@ -3042,7 +3405,10 @@
         <v>241</v>
       </c>
     </row>
-    <row r="124" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A124" s="7" t="s">
+        <v>315</v>
+      </c>
       <c r="B124" s="8" t="s">
         <v>244</v>
       </c>
@@ -3056,7 +3422,10 @@
         <v>243</v>
       </c>
     </row>
-    <row r="125" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A125" s="7" t="s">
+        <v>319</v>
+      </c>
       <c r="B125" s="8" t="s">
         <v>246</v>
       </c>
@@ -3070,7 +3439,10 @@
         <v>245</v>
       </c>
     </row>
-    <row r="126" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A126" s="7" t="s">
+        <v>319</v>
+      </c>
       <c r="B126" s="8" t="s">
         <v>248</v>
       </c>
@@ -3084,7 +3456,10 @@
         <v>247</v>
       </c>
     </row>
-    <row r="127" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A127" s="7" t="s">
+        <v>319</v>
+      </c>
       <c r="B127" s="8" t="s">
         <v>250</v>
       </c>
@@ -3098,7 +3473,10 @@
         <v>249</v>
       </c>
     </row>
-    <row r="128" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A128" s="7" t="s">
+        <v>304</v>
+      </c>
       <c r="B128" s="8" t="s">
         <v>252</v>
       </c>
@@ -3115,7 +3493,10 @@
       <c r="I128" s="5"/>
       <c r="J128" s="4"/>
     </row>
-    <row r="129" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A129" s="7" t="s">
+        <v>304</v>
+      </c>
       <c r="B129" s="8" t="s">
         <v>254</v>
       </c>

</xml_diff>